<commit_message>
interventions page working, but going to remove number column
</commit_message>
<xml_diff>
--- a/data/interventions-demo.xlsx
+++ b/data/interventions-demo.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="18" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$B$1:$Z$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$C$1:$AA$30</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="190">
   <si>
     <t>Community</t>
   </si>
@@ -589,6 +589,9 @@
   </si>
   <si>
     <t>Implemented?</t>
+  </si>
+  <si>
+    <t>Active</t>
   </si>
 </sst>
 </file>
@@ -1730,31 +1733,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="462" builtinId="5"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="31">
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -2076,6 +2055,54 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFF5F1E3"/>
@@ -2096,8 +2123,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7">
     <tableStyle name="Table Style 1" pivot="0" count="2">
-      <tableStyleElement type="headerRow" dxfId="29"/>
-      <tableStyleElement type="firstRowStripe" dxfId="28"/>
+      <tableStyleElement type="headerRow" dxfId="30"/>
+      <tableStyleElement type="firstRowStripe" dxfId="29"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2121,35 +2148,36 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Z31" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A1:Z31"/>
-  <tableColumns count="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AA31" totalsRowShown="0" headerRowDxfId="28" dataDxfId="0">
+  <autoFilter ref="A1:AA31"/>
+  <tableColumns count="27">
     <tableColumn id="1" name="No." dataDxfId="27"/>
-    <tableColumn id="2" name="Full name" dataDxfId="26"/>
-    <tableColumn id="3" name="Short name" dataDxfId="25"/>
-    <tableColumn id="4" name="Platform" dataDxfId="24"/>
-    <tableColumn id="5" name="BoD (1)" dataDxfId="23"/>
-    <tableColumn id="6" name="Fraction (1)" dataDxfId="22"/>
-    <tableColumn id="7" name="BoD (2)" dataDxfId="21"/>
-    <tableColumn id="8" name="Fraction (2)" dataDxfId="20"/>
-    <tableColumn id="9" name="BoD (3)" dataDxfId="19"/>
-    <tableColumn id="10" name="Fraction (3)" dataDxfId="18"/>
-    <tableColumn id="11" name="ICER" dataDxfId="17" dataCellStyle="Comma"/>
-    <tableColumn id="12" name="Unit cost" dataDxfId="16" dataCellStyle="Comma"/>
-    <tableColumn id="13" name="Spending" dataDxfId="15" dataCellStyle="Comma"/>
-    <tableColumn id="14" name="FRP" dataDxfId="14"/>
-    <tableColumn id="15" name="Equity" dataDxfId="13"/>
-    <tableColumn id="16" name="HPP" dataDxfId="12"/>
-    <tableColumn id="17" name="DCP3 packages" dataDxfId="11"/>
-    <tableColumn id="18" name="Package number" dataDxfId="10"/>
-    <tableColumn id="19" name="DCP number" dataDxfId="9"/>
-    <tableColumn id="20" name="Urgency" dataDxfId="8"/>
-    <tableColumn id="21" name="Implemented?" dataDxfId="7"/>
-    <tableColumn id="22" name="Outcome measured" dataDxfId="6"/>
-    <tableColumn id="23" name="Relative risk (RR)" dataDxfId="5"/>
-    <tableColumn id="24" name="RR (lower)" dataDxfId="4"/>
-    <tableColumn id="25" name="RR (upper)" dataDxfId="3"/>
-    <tableColumn id="26" name="Coverage" dataDxfId="2" dataCellStyle="Percent"/>
+    <tableColumn id="27" name="Active" dataDxfId="26"/>
+    <tableColumn id="2" name="Full name" dataDxfId="25"/>
+    <tableColumn id="3" name="Short name" dataDxfId="24"/>
+    <tableColumn id="4" name="Platform" dataDxfId="23"/>
+    <tableColumn id="5" name="BoD (1)" dataDxfId="22"/>
+    <tableColumn id="6" name="Fraction (1)" dataDxfId="21"/>
+    <tableColumn id="7" name="BoD (2)" dataDxfId="20"/>
+    <tableColumn id="8" name="Fraction (2)" dataDxfId="19"/>
+    <tableColumn id="9" name="BoD (3)" dataDxfId="18"/>
+    <tableColumn id="10" name="Fraction (3)" dataDxfId="17"/>
+    <tableColumn id="11" name="ICER" dataDxfId="16" dataCellStyle="Comma"/>
+    <tableColumn id="12" name="Unit cost" dataDxfId="15" dataCellStyle="Comma"/>
+    <tableColumn id="13" name="Spending" dataDxfId="14" dataCellStyle="Comma"/>
+    <tableColumn id="14" name="FRP" dataDxfId="13"/>
+    <tableColumn id="15" name="Equity" dataDxfId="12"/>
+    <tableColumn id="16" name="HPP" dataDxfId="11"/>
+    <tableColumn id="17" name="DCP3 packages" dataDxfId="10"/>
+    <tableColumn id="18" name="Package number" dataDxfId="9"/>
+    <tableColumn id="19" name="DCP number" dataDxfId="8"/>
+    <tableColumn id="20" name="Urgency" dataDxfId="7"/>
+    <tableColumn id="21" name="Implemented?" dataDxfId="6"/>
+    <tableColumn id="22" name="Outcome measured" dataDxfId="5"/>
+    <tableColumn id="23" name="Relative risk (RR)" dataDxfId="4"/>
+    <tableColumn id="24" name="RR (lower)" dataDxfId="3"/>
+    <tableColumn id="25" name="RR (upper)" dataDxfId="2"/>
+    <tableColumn id="26" name="Coverage" dataDxfId="1" dataCellStyle="Percent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2410,7 +2438,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2418,2210 +2446,2353 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA31"/>
+  <dimension ref="A1:AB31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q18" sqref="Q18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="68.875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="40" style="2" customWidth="1"/>
-    <col min="4" max="4" width="18.5" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25.625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
-    <col min="7" max="7" width="21.875" style="9" customWidth="1"/>
-    <col min="8" max="10" width="12.5" style="9" customWidth="1"/>
-    <col min="11" max="11" width="22.625" style="7" customWidth="1"/>
-    <col min="12" max="12" width="14.625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="8.625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="76.75" style="2" customWidth="1"/>
+    <col min="4" max="4" width="32.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19.5" style="9" customWidth="1"/>
+    <col min="6" max="6" width="29" style="9" customWidth="1"/>
+    <col min="7" max="7" width="13.625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="25.625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="12.5" style="9" customWidth="1"/>
+    <col min="10" max="10" width="24.375" style="9" customWidth="1"/>
+    <col min="11" max="11" width="13.5" style="7" customWidth="1"/>
+    <col min="12" max="12" width="8.625" style="11" customWidth="1"/>
     <col min="13" max="13" width="11.5" style="7" customWidth="1"/>
-    <col min="14" max="14" width="6.625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="12" style="2" customWidth="1"/>
+    <col min="14" max="14" width="12.5" style="2" customWidth="1"/>
+    <col min="15" max="15" width="7.125" style="2" customWidth="1"/>
     <col min="16" max="16" width="9.625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="32.875" style="2" customWidth="1"/>
-    <col min="18" max="18" width="20.125" style="3" customWidth="1"/>
-    <col min="19" max="19" width="14.375" style="2" customWidth="1"/>
-    <col min="20" max="20" width="11.875" style="2" customWidth="1"/>
-    <col min="21" max="21" width="14.875" style="2" customWidth="1"/>
-    <col min="22" max="22" width="26.5" style="9" customWidth="1"/>
-    <col min="23" max="23" width="17.5" style="2" customWidth="1"/>
-    <col min="24" max="24" width="13.75" style="2" customWidth="1"/>
+    <col min="17" max="17" width="7.625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="31.375" style="3" customWidth="1"/>
+    <col min="19" max="19" width="20.25" style="2" customWidth="1"/>
+    <col min="20" max="21" width="14.875" style="2" customWidth="1"/>
+    <col min="22" max="22" width="17.25" style="9" customWidth="1"/>
+    <col min="23" max="23" width="37.125" style="2" customWidth="1"/>
+    <col min="24" max="24" width="18.5" style="2" customWidth="1"/>
     <col min="25" max="25" width="14.75" style="2" customWidth="1"/>
     <col min="26" max="26" width="11.875" style="17" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="11.875" style="17" customWidth="1"/>
     <col min="28" max="16384" width="8.875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:28" ht="32.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>180</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="D1" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="E1" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>169</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>168</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="I1" s="20" t="s">
         <v>171</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="J1" s="20" t="s">
         <v>172</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="K1" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>174</v>
       </c>
-      <c r="L1" s="22" t="s">
+      <c r="M1" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="N1" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="O1" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="P1" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="Q1" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="Q1" s="20" t="s">
+      <c r="R1" s="20" t="s">
         <v>185</v>
       </c>
-      <c r="R1" s="23" t="s">
+      <c r="S1" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="S1" s="20" t="s">
+      <c r="T1" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="T1" s="20" t="s">
+      <c r="U1" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="U1" s="20" t="s">
+      <c r="V1" s="20" t="s">
         <v>188</v>
       </c>
-      <c r="V1" s="20" t="s">
+      <c r="W1" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="W1" s="20" t="s">
+      <c r="X1" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="X1" s="20" t="s">
+      <c r="Y1" s="20" t="s">
         <v>183</v>
       </c>
-      <c r="Y1" s="20" t="s">
+      <c r="Z1" s="20" t="s">
         <v>184</v>
       </c>
-      <c r="Z1" s="20" t="s">
+      <c r="AA1" s="20" t="s">
         <v>147</v>
       </c>
-      <c r="AA1" s="15"/>
+      <c r="AB1" s="15"/>
     </row>
-    <row r="2" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="F2" s="9">
+      <c r="G2" s="9">
         <v>0.7</v>
       </c>
-      <c r="K2" s="8">
+      <c r="K2" s="9"/>
+      <c r="L2" s="8">
         <v>7</v>
       </c>
-      <c r="L2" s="11">
+      <c r="M2" s="11">
         <v>0.78435308805910964</v>
       </c>
-      <c r="M2" s="7">
+      <c r="N2" s="7">
         <v>2249.183019582937</v>
       </c>
-      <c r="N2" s="2">
+      <c r="O2" s="2">
         <v>5</v>
       </c>
-      <c r="O2" s="2">
+      <c r="P2" s="2">
         <v>3</v>
       </c>
-      <c r="P2" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="2">
+        <v>1</v>
+      </c>
+      <c r="R2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="R2" s="5">
-        <v>1</v>
-      </c>
-      <c r="S2" s="9" t="s">
+      <c r="S2" s="5">
+        <v>1</v>
+      </c>
+      <c r="T2" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="U2" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="U2" s="2">
-        <v>1</v>
-      </c>
-      <c r="V2" s="9" t="s">
+      <c r="V2" s="2">
+        <v>1</v>
+      </c>
+      <c r="W2" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="W2" s="2">
+      <c r="X2" s="2">
         <v>0.41</v>
       </c>
-      <c r="X2" s="2">
+      <c r="Y2" s="2">
         <v>0.28999999999999998</v>
       </c>
-      <c r="Y2" s="2">
+      <c r="Z2" s="2">
         <v>0.57999999999999996</v>
       </c>
-      <c r="Z2" s="17">
+      <c r="AA2" s="17">
         <f>0.210614324578582*(0.88)</f>
         <v>0.18534060562915217</v>
       </c>
+      <c r="AB2" s="17"/>
     </row>
-    <row r="3" spans="1:27" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" s="18" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="18">
         <v>2</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>6</v>
+      <c r="B3" s="18">
+        <v>1</v>
       </c>
       <c r="C3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="F3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="13">
+      <c r="G3" s="13">
         <v>0.05</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="H3" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="H3" s="13">
+      <c r="I3" s="13">
         <v>0.5</v>
       </c>
-      <c r="I3" s="13"/>
       <c r="J3" s="13"/>
-      <c r="K3" s="14">
+      <c r="K3" s="13"/>
+      <c r="L3" s="14">
         <v>250</v>
       </c>
-      <c r="L3" s="11">
+      <c r="M3" s="11">
         <v>254.60902660160465</v>
       </c>
-      <c r="M3" s="7">
+      <c r="N3" s="7">
         <v>3533205.6138780504</v>
       </c>
-      <c r="N3" s="4">
+      <c r="O3" s="4">
         <v>5</v>
       </c>
-      <c r="O3" s="4">
-        <v>1</v>
-      </c>
       <c r="P3" s="4">
         <v>1</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Q3" s="4">
+        <v>1</v>
+      </c>
+      <c r="R3" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="S3" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="S3" s="13" t="s">
+      <c r="T3" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="T3" s="4" t="s">
+      <c r="U3" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="U3" s="4">
-        <v>1</v>
-      </c>
-      <c r="V3" s="13"/>
-      <c r="W3" s="4"/>
+      <c r="V3" s="4">
+        <v>1</v>
+      </c>
+      <c r="W3" s="13"/>
       <c r="X3" s="4"/>
       <c r="Y3" s="4"/>
-      <c r="Z3" s="17">
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="17">
         <v>0.4</v>
       </c>
-      <c r="AA3" s="17"/>
+      <c r="AB3" s="17"/>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
+      <c r="B4" s="2">
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="F4" s="2">
+      <c r="G4" s="2">
         <v>0.3</v>
       </c>
-      <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="2">
+      <c r="K4" s="2"/>
+      <c r="L4" s="2">
         <v>11</v>
       </c>
-      <c r="L4" s="11">
+      <c r="M4" s="11">
         <v>1.2581054540850005</v>
       </c>
-      <c r="M4" s="7">
+      <c r="N4" s="7">
         <v>547.48769225846445</v>
       </c>
-      <c r="N4" s="2">
+      <c r="O4" s="2">
         <v>6</v>
       </c>
-      <c r="O4" s="2">
-        <v>1</v>
-      </c>
       <c r="P4" s="2">
         <v>1</v>
       </c>
-      <c r="Q4" s="4" t="s">
+      <c r="Q4" s="2">
+        <v>1</v>
+      </c>
+      <c r="R4" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="R4" s="5">
+      <c r="S4" s="5">
         <v>18</v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="T4" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="T4" s="4" t="s">
+      <c r="U4" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="U4" s="4">
-        <v>1</v>
-      </c>
-      <c r="V4" s="2" t="s">
+      <c r="V4" s="4">
+        <v>1</v>
+      </c>
+      <c r="W4" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="W4" s="2">
+      <c r="X4" s="2">
         <v>0.31200000000000006</v>
-      </c>
-      <c r="X4" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="Y4" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="Z4" s="17">
+      <c r="Z4" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA4" s="17">
         <f>0.1*(0.88)</f>
         <v>8.8000000000000009E-2</v>
       </c>
+      <c r="AB4" s="17"/>
     </row>
-    <row r="5" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="18">
         <v>4</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="18">
+        <v>1</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="D5" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="F5" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="9">
+      <c r="G5" s="9">
         <v>0.8</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="9"/>
+      <c r="L5" s="8">
         <v>13</v>
       </c>
-      <c r="L5" s="11">
+      <c r="M5" s="11">
         <v>2.0230000000000001E-2</v>
       </c>
-      <c r="M5" s="7">
+      <c r="N5" s="7">
         <v>193.21521892743283</v>
       </c>
-      <c r="N5" s="2">
+      <c r="O5" s="2">
         <v>2</v>
       </c>
-      <c r="O5" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="2" t="s">
+      <c r="P5" s="2">
+        <v>1</v>
+      </c>
+      <c r="R5" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="R5" s="3">
+      <c r="S5" s="3">
         <v>8</v>
       </c>
-      <c r="S5" s="9" t="s">
+      <c r="T5" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="T5" s="2" t="s">
+      <c r="U5" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="U5" s="2">
-        <v>1</v>
-      </c>
-      <c r="V5" s="9" t="s">
+      <c r="V5" s="2">
+        <v>1</v>
+      </c>
+      <c r="W5" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="W5" s="2">
+      <c r="X5" s="2">
         <v>0.12</v>
       </c>
-      <c r="X5" s="2">
+      <c r="Y5" s="2">
         <v>0.02</v>
       </c>
-      <c r="Y5" s="2">
+      <c r="Z5" s="2">
         <v>0.88</v>
       </c>
-      <c r="Z5" s="17">
+      <c r="AA5" s="17">
         <v>0.4</v>
       </c>
+      <c r="AB5" s="17"/>
     </row>
-    <row r="6" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="F6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="9">
+      <c r="G6" s="9">
         <v>0.8</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="9"/>
+      <c r="L6" s="8">
         <v>13</v>
       </c>
-      <c r="L6" s="11">
+      <c r="M6" s="11">
         <v>1.7790273640275014</v>
       </c>
-      <c r="M6" s="7">
+      <c r="N6" s="7">
         <v>16991.35747001816</v>
       </c>
-      <c r="N6" s="2">
-        <v>1</v>
-      </c>
       <c r="O6" s="2">
         <v>1</v>
       </c>
-      <c r="Q6" s="2" t="s">
+      <c r="P6" s="2">
+        <v>1</v>
+      </c>
+      <c r="R6" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="R6" s="3">
+      <c r="S6" s="3">
         <v>8</v>
       </c>
-      <c r="S6" s="9" t="s">
+      <c r="T6" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="T6" s="2" t="s">
+      <c r="U6" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="U6" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z6" s="17">
+      <c r="V6" s="2">
+        <v>1</v>
+      </c>
+      <c r="W6" s="9"/>
+      <c r="Z6" s="2"/>
+      <c r="AA6" s="17">
         <v>0.4</v>
       </c>
+      <c r="AB6" s="17"/>
     </row>
-    <row r="7" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="18">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>16</v>
+      <c r="B7" s="18">
+        <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="F7" s="2">
+      <c r="G7" s="2">
         <v>0.2</v>
       </c>
-      <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
-      <c r="K7" s="2">
+      <c r="K7" s="2"/>
+      <c r="L7" s="2">
         <v>13</v>
       </c>
-      <c r="L7" s="11">
+      <c r="M7" s="11">
         <v>1.2581054540850005</v>
       </c>
-      <c r="M7" s="7">
+      <c r="N7" s="7">
         <v>36317.200212839991</v>
       </c>
-      <c r="N7" s="2">
+      <c r="O7" s="2">
         <v>5</v>
       </c>
-      <c r="O7" s="2">
+      <c r="P7" s="2">
         <v>3</v>
       </c>
-      <c r="P7" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="2" t="s">
+      <c r="Q7" s="2">
+        <v>1</v>
+      </c>
+      <c r="R7" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="R7" s="3">
+      <c r="S7" s="3">
         <v>11</v>
       </c>
-      <c r="S7" s="2" t="s">
+      <c r="T7" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="T7" s="2" t="s">
+      <c r="U7" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="U7" s="2">
-        <v>1</v>
-      </c>
-      <c r="V7" s="2" t="s">
+      <c r="V7" s="2">
+        <v>1</v>
+      </c>
+      <c r="W7" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="W7" s="2">
+      <c r="X7" s="2">
         <v>0.66</v>
       </c>
-      <c r="X7" s="2">
+      <c r="Y7" s="2">
         <v>0.48</v>
       </c>
-      <c r="Y7" s="2">
+      <c r="Z7" s="2">
         <v>0.89</v>
       </c>
-      <c r="Z7" s="17">
+      <c r="AA7" s="17">
         <f>0.1*(0.88)</f>
         <v>8.8000000000000009E-2</v>
       </c>
+      <c r="AB7" s="17"/>
     </row>
-    <row r="8" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="2">
+        <v>1</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="D8" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="F8" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="F8" s="2">
+      <c r="G8" s="2">
         <v>0.1</v>
       </c>
-      <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2"/>
-      <c r="K8" s="8">
+      <c r="K8" s="2"/>
+      <c r="L8" s="8">
         <v>14</v>
       </c>
-      <c r="L8" s="11">
+      <c r="M8" s="11">
         <v>48.128585671910834</v>
       </c>
-      <c r="M8" s="6">
+      <c r="N8" s="6">
         <v>19671.661741774085</v>
       </c>
-      <c r="N8" s="1">
+      <c r="O8" s="1">
         <v>4</v>
       </c>
-      <c r="O8" s="1">
+      <c r="P8" s="1">
         <v>3</v>
       </c>
-      <c r="P8" s="1">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="2" t="s">
+      <c r="Q8" s="1">
+        <v>1</v>
+      </c>
+      <c r="R8" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="R8" s="3">
-        <v>1</v>
-      </c>
-      <c r="S8" s="9" t="s">
+      <c r="S8" s="3">
+        <v>1</v>
+      </c>
+      <c r="T8" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="T8" s="2" t="s">
+      <c r="U8" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="U8" s="2">
-        <v>1</v>
-      </c>
-      <c r="V8" s="2" t="s">
+      <c r="V8" s="2">
+        <v>1</v>
+      </c>
+      <c r="W8" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="W8" s="2">
+      <c r="X8" s="2">
         <v>0.8</v>
       </c>
-      <c r="X8" s="2">
+      <c r="Y8" s="2">
         <v>0.5</v>
       </c>
-      <c r="Y8" s="2">
+      <c r="Z8" s="2">
         <v>0.9</v>
       </c>
-      <c r="Z8" s="17">
+      <c r="AA8" s="17">
         <f>0.068635045612025*(0.88)</f>
         <v>6.0398840138582002E-2</v>
       </c>
+      <c r="AB8" s="17"/>
     </row>
-    <row r="9" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="18">
         <v>8</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="18">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="D9" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="F9" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="9">
+      <c r="G9" s="9">
         <v>0.2</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9" s="9"/>
+      <c r="L9" s="8">
         <v>20</v>
       </c>
-      <c r="L9" s="11">
+      <c r="M9" s="11">
         <v>1.2581054540850005</v>
       </c>
-      <c r="M9" s="7">
+      <c r="N9" s="7">
         <v>165691.53429320332</v>
       </c>
-      <c r="N9" s="2">
+      <c r="O9" s="2">
         <v>3</v>
       </c>
-      <c r="O9" s="2">
-        <v>1</v>
-      </c>
       <c r="P9" s="2">
         <v>1</v>
       </c>
-      <c r="Q9" s="2" t="s">
+      <c r="Q9" s="2">
+        <v>1</v>
+      </c>
+      <c r="R9" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="R9" s="3">
+      <c r="S9" s="3">
         <v>11</v>
       </c>
-      <c r="S9" s="9" t="s">
+      <c r="T9" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="T9" s="2" t="s">
+      <c r="U9" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="U9" s="2">
-        <v>1</v>
-      </c>
-      <c r="V9" s="9" t="s">
+      <c r="V9" s="2">
+        <v>1</v>
+      </c>
+      <c r="W9" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="W9" s="2">
+      <c r="X9" s="2">
         <v>3.7000000000000002E-3</v>
       </c>
-      <c r="X9" s="2">
+      <c r="Y9" s="2">
         <v>2.8E-3</v>
       </c>
-      <c r="Y9" s="2">
+      <c r="Z9" s="2">
         <v>4.4999999999999997E-3</v>
       </c>
-      <c r="Z9" s="17">
+      <c r="AA9" s="17">
         <f>0.1*(0.88)</f>
         <v>8.8000000000000009E-2</v>
       </c>
+      <c r="AB9" s="17"/>
     </row>
-    <row r="10" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>2</v>
+      <c r="B10" s="2">
+        <v>1</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="F10" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="F10" s="9">
+      <c r="G10" s="9">
         <v>0.4</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10" s="9"/>
+      <c r="L10" s="8">
         <v>22</v>
       </c>
-      <c r="L10" s="11">
+      <c r="M10" s="11">
         <v>1.6708715227994324</v>
       </c>
-      <c r="M10" s="7">
+      <c r="N10" s="7">
         <v>3963955.5316596483</v>
       </c>
-      <c r="N10" s="2">
+      <c r="O10" s="2">
         <v>3</v>
       </c>
-      <c r="O10" s="2">
-        <v>1</v>
-      </c>
       <c r="P10" s="2">
         <v>1</v>
       </c>
-      <c r="Q10" s="4" t="s">
+      <c r="Q10" s="2">
+        <v>1</v>
+      </c>
+      <c r="R10" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="R10" s="5">
+      <c r="S10" s="5">
         <v>18</v>
       </c>
-      <c r="S10" s="9" t="s">
+      <c r="T10" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="T10" s="4" t="s">
+      <c r="U10" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="U10" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z10" s="17">
+      <c r="V10" s="2">
+        <v>1</v>
+      </c>
+      <c r="W10" s="9"/>
+      <c r="Z10" s="2"/>
+      <c r="AA10" s="17">
         <f>0.306720966623047*(0.88)</f>
         <v>0.26991445062828134</v>
       </c>
+      <c r="AB10" s="17"/>
     </row>
-    <row r="11" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="18">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="18">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="F11" s="9">
+      <c r="G11" s="9">
         <v>0.85</v>
       </c>
-      <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="2">
+      <c r="K11" s="2"/>
+      <c r="L11" s="2">
         <v>23</v>
       </c>
-      <c r="L11" s="11">
+      <c r="M11" s="11">
         <v>1.1496900605005875</v>
       </c>
-      <c r="M11" s="7">
+      <c r="N11" s="7">
         <v>61220.64852115501</v>
       </c>
-      <c r="N11" s="2">
+      <c r="O11" s="2">
         <v>4</v>
       </c>
-      <c r="O11" s="2">
-        <v>1</v>
-      </c>
       <c r="P11" s="2">
         <v>1</v>
       </c>
-      <c r="Q11" s="2" t="s">
+      <c r="Q11" s="2">
+        <v>1</v>
+      </c>
+      <c r="R11" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="R11" s="3">
+      <c r="S11" s="3">
         <v>14</v>
       </c>
-      <c r="S11" s="2" t="s">
+      <c r="T11" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="T11" s="2" t="s">
+      <c r="U11" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="U11" s="2">
-        <v>1</v>
-      </c>
-      <c r="V11" s="2" t="s">
+      <c r="V11" s="2">
+        <v>1</v>
+      </c>
+      <c r="W11" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="W11" s="2">
+      <c r="X11" s="2">
         <v>4.8</v>
       </c>
-      <c r="X11" s="2">
+      <c r="Y11" s="2">
         <v>0.7</v>
       </c>
-      <c r="Y11" s="2">
+      <c r="Z11" s="2">
         <v>8.9</v>
       </c>
-      <c r="Z11" s="17">
+      <c r="AA11" s="17">
         <f>0.924908816360775*(0.88)</f>
         <v>0.8139197583974821</v>
       </c>
+      <c r="AB11" s="17"/>
     </row>
-    <row r="12" spans="1:27" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="D12" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="F12" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="9">
+      <c r="G12" s="9">
         <v>0.05</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="H12" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="H12" s="9">
+      <c r="I12" s="9">
         <v>0.03</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="J12" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="J12" s="9">
+      <c r="K12" s="9">
         <v>0.02</v>
       </c>
-      <c r="K12" s="8">
+      <c r="L12" s="8">
         <v>28</v>
       </c>
-      <c r="L12" s="11">
+      <c r="M12" s="11">
         <v>4.819458994482523</v>
       </c>
-      <c r="M12" s="7">
+      <c r="N12" s="7">
         <v>1623532.4666199405</v>
       </c>
-      <c r="N12" s="2">
+      <c r="O12" s="2">
         <v>3</v>
       </c>
-      <c r="O12" s="2">
-        <v>1</v>
-      </c>
       <c r="P12" s="2">
         <v>1</v>
       </c>
-      <c r="Q12" s="2" t="s">
+      <c r="Q12" s="2">
+        <v>1</v>
+      </c>
+      <c r="R12" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="R12" s="3">
+      <c r="S12" s="3">
         <v>6</v>
       </c>
-      <c r="S12" s="9" t="s">
+      <c r="T12" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="T12" s="2" t="s">
+      <c r="U12" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="U12" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z12" s="17">
+      <c r="V12" s="2">
+        <v>1</v>
+      </c>
+      <c r="W12" s="9"/>
+      <c r="Z12" s="2"/>
+      <c r="AA12" s="17">
         <f>0.104473979264733*(0.88)</f>
         <v>9.1937101752965031E-2</v>
       </c>
+      <c r="AB12" s="17"/>
     </row>
-    <row r="13" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="18">
         <v>12</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="18">
+        <v>1</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="D13" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="F13" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F13" s="9">
+      <c r="G13" s="9">
         <v>0.4</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K13" s="9"/>
+      <c r="L13" s="8">
         <v>31</v>
       </c>
-      <c r="L13" s="11">
+      <c r="M13" s="11">
         <v>1.344397990175465</v>
       </c>
-      <c r="M13" s="7">
+      <c r="N13" s="7">
         <v>8235.4710468978228</v>
       </c>
-      <c r="N13" s="2">
+      <c r="O13" s="2">
         <v>3</v>
       </c>
-      <c r="O13" s="2">
-        <v>1</v>
-      </c>
       <c r="P13" s="2">
         <v>1</v>
       </c>
-      <c r="Q13" s="2" t="s">
+      <c r="Q13" s="2">
+        <v>1</v>
+      </c>
+      <c r="R13" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="R13" s="3">
+      <c r="S13" s="3">
         <v>8</v>
       </c>
-      <c r="S13" s="9" t="s">
+      <c r="T13" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="T13" s="2" t="s">
+      <c r="U13" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="U13" s="2">
-        <v>1</v>
-      </c>
-      <c r="V13" s="2" t="s">
+      <c r="V13" s="2">
+        <v>1</v>
+      </c>
+      <c r="W13" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="W13" s="2">
+      <c r="X13" s="2">
         <v>0.57999999999999996</v>
       </c>
-      <c r="X13" s="2">
+      <c r="Y13" s="2">
         <v>0.44</v>
       </c>
-      <c r="Y13" s="2">
+      <c r="Z13" s="2">
         <v>0.77</v>
       </c>
-      <c r="Z13" s="17">
+      <c r="AA13" s="17">
         <f>0.291536181212621*(0.88)</f>
         <v>0.25655183946710647</v>
       </c>
+      <c r="AB13" s="17"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="2">
+        <v>1</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="D14" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="F14" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="F14" s="9">
+      <c r="G14" s="9">
         <v>0.4</v>
       </c>
-      <c r="K14" s="14">
-        <f>K17</f>
+      <c r="K14" s="9"/>
+      <c r="L14" s="14">
+        <f>L17</f>
         <v>103</v>
       </c>
-      <c r="L14" s="11">
+      <c r="M14" s="11">
         <v>19.359239841281244</v>
       </c>
-      <c r="M14" s="7">
+      <c r="N14" s="7">
         <v>116615.41965520391</v>
       </c>
-      <c r="N14" s="2">
+      <c r="O14" s="2">
         <v>3</v>
       </c>
-      <c r="O14" s="2">
-        <v>1</v>
-      </c>
       <c r="P14" s="2">
         <v>1</v>
       </c>
-      <c r="Q14" s="2" t="s">
+      <c r="Q14" s="2">
+        <v>1</v>
+      </c>
+      <c r="R14" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="R14" s="3">
-        <v>1</v>
-      </c>
-      <c r="S14" s="9" t="s">
+      <c r="S14" s="3">
+        <v>1</v>
+      </c>
+      <c r="T14" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="T14" s="2" t="s">
+      <c r="U14" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="U14" s="2">
-        <v>1</v>
-      </c>
-      <c r="V14" s="12" t="s">
+      <c r="V14" s="2">
+        <v>1</v>
+      </c>
+      <c r="W14" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="W14" s="2">
+      <c r="X14" s="2">
         <v>0.57999999999999996</v>
       </c>
-      <c r="X14" s="2">
+      <c r="Y14" s="2">
         <v>0.41</v>
       </c>
-      <c r="Y14" s="2">
+      <c r="Z14" s="2">
         <v>0.82</v>
       </c>
-      <c r="Z14" s="17">
+      <c r="AA14" s="17">
         <f>0.253110379496502*(0.88)</f>
         <v>0.22273713395692177</v>
       </c>
+      <c r="AB14" s="17"/>
     </row>
-    <row r="15" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="18">
         <v>14</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="18">
+        <v>1</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="D15" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="F15" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="F15" s="9">
+      <c r="G15" s="9">
         <v>0.2</v>
       </c>
-      <c r="G15" s="9" t="s">
+      <c r="H15" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="H15" s="9">
+      <c r="I15" s="9">
         <v>0.6</v>
       </c>
-      <c r="K15" s="14">
-        <f>K24</f>
+      <c r="K15" s="9"/>
+      <c r="L15" s="14">
+        <f>L24</f>
         <v>576</v>
       </c>
-      <c r="L15" s="11">
+      <c r="M15" s="11">
         <v>7.4900031183195228</v>
       </c>
-      <c r="M15" s="7">
+      <c r="N15" s="7">
         <v>17032516.326998692</v>
       </c>
-      <c r="N15" s="2">
+      <c r="O15" s="2">
         <v>3</v>
       </c>
-      <c r="O15" s="2">
-        <v>1</v>
-      </c>
       <c r="P15" s="2">
         <v>1</v>
       </c>
-      <c r="Q15" s="2" t="s">
+      <c r="Q15" s="2">
+        <v>1</v>
+      </c>
+      <c r="R15" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="R15" s="3" t="s">
+      <c r="S15" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="S15" s="9" t="s">
+      <c r="T15" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="T15" s="2" t="s">
+      <c r="U15" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="U15" s="2">
-        <v>1</v>
-      </c>
-      <c r="V15" s="9" t="s">
+      <c r="V15" s="2">
+        <v>1</v>
+      </c>
+      <c r="W15" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="W15" s="2">
+      <c r="X15" s="2">
         <v>0.5</v>
       </c>
-      <c r="X15" s="2">
+      <c r="Y15" s="2">
         <v>0.3</v>
       </c>
-      <c r="Y15" s="2">
+      <c r="Z15" s="2">
         <v>0.9</v>
       </c>
-      <c r="Z15" s="17">
+      <c r="AA15" s="17">
         <f>0.708210560611961*(0.88)</f>
         <v>0.62322529333852561</v>
       </c>
+      <c r="AB15" s="17"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="F16" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="F16" s="2">
+      <c r="G16" s="2">
         <v>0.3</v>
       </c>
-      <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
-      <c r="K16" s="2">
+      <c r="K16" s="2"/>
+      <c r="L16" s="2">
         <v>95</v>
       </c>
-      <c r="L16" s="11">
+      <c r="M16" s="11">
         <v>216.54621737662529</v>
       </c>
-      <c r="M16" s="7">
+      <c r="N16" s="7">
         <v>16215973.791515743</v>
       </c>
-      <c r="N16" s="2">
+      <c r="O16" s="2">
         <v>3</v>
       </c>
-      <c r="O16" s="2">
-        <v>1</v>
-      </c>
       <c r="P16" s="2">
         <v>1</v>
       </c>
-      <c r="Q16" s="2" t="s">
+      <c r="Q16" s="2">
+        <v>1</v>
+      </c>
+      <c r="R16" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="R16" s="3">
+      <c r="S16" s="3">
         <v>2</v>
       </c>
-      <c r="S16" s="2" t="s">
+      <c r="T16" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="T16" s="2" t="s">
+      <c r="U16" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="U16" s="2">
-        <v>1</v>
-      </c>
-      <c r="V16" s="2" t="s">
+      <c r="V16" s="2">
+        <v>1</v>
+      </c>
+      <c r="W16" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="W16" s="2">
+      <c r="X16" s="2">
         <v>0.7</v>
       </c>
-      <c r="X16" s="2">
+      <c r="Y16" s="2">
         <v>0.57999999999999996</v>
       </c>
-      <c r="Y16" s="2">
+      <c r="Z16" s="2">
         <v>0.85</v>
       </c>
-      <c r="Z16" s="17">
+      <c r="AA16" s="17">
         <f>0.14396030496079*(0.88)</f>
         <v>0.1266850683654952</v>
       </c>
+      <c r="AB16" s="17"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="18">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>29</v>
+      <c r="B17" s="18">
+        <v>1</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="F17" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="F17" s="2">
+      <c r="G17" s="2">
         <v>0.7</v>
       </c>
-      <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
-      <c r="K17" s="2">
+      <c r="K17" s="2"/>
+      <c r="L17" s="2">
         <v>103</v>
       </c>
-      <c r="L17" s="11">
+      <c r="M17" s="11">
         <v>1.2581054540850005</v>
       </c>
-      <c r="M17" s="6">
+      <c r="N17" s="6">
         <v>17964.950282769361</v>
-      </c>
-      <c r="N17" s="2">
-        <v>2</v>
       </c>
       <c r="O17" s="2">
         <v>2</v>
       </c>
       <c r="P17" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>1</v>
+      </c>
+      <c r="R17" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="R17" s="3">
+      <c r="S17" s="3">
         <v>2</v>
       </c>
-      <c r="S17" s="2" t="s">
+      <c r="T17" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="T17" s="2" t="s">
+      <c r="U17" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="U17" s="2">
-        <v>1</v>
-      </c>
-      <c r="V17" s="2" t="s">
+      <c r="V17" s="2">
+        <v>1</v>
+      </c>
+      <c r="W17" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="W17" s="2">
+      <c r="X17" s="2">
         <v>0.57999999999999996</v>
       </c>
-      <c r="X17" s="2">
+      <c r="Y17" s="2">
         <v>0.18</v>
       </c>
-      <c r="Y17" s="2">
+      <c r="Z17" s="2">
         <v>1.9</v>
       </c>
-      <c r="Z17" s="17">
+      <c r="AA17" s="17">
         <f>0.6*(0.88)</f>
         <v>0.52800000000000002</v>
       </c>
+      <c r="AB17" s="17"/>
     </row>
-    <row r="18" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="D18" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="F18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="9">
+      <c r="G18" s="9">
         <v>0.4</v>
       </c>
-      <c r="K18" s="8">
+      <c r="K18" s="9"/>
+      <c r="L18" s="8">
         <v>115</v>
       </c>
-      <c r="L18" s="11">
+      <c r="M18" s="11">
         <v>21.299447386134773</v>
       </c>
-      <c r="M18" s="7">
+      <c r="N18" s="7">
         <v>325775.66857809632</v>
       </c>
-      <c r="N18" s="2">
+      <c r="O18" s="2">
         <v>4</v>
       </c>
-      <c r="O18" s="2">
+      <c r="P18" s="2">
         <v>3</v>
       </c>
-      <c r="P18" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="2" t="s">
+      <c r="Q18" s="2">
+        <v>1</v>
+      </c>
+      <c r="R18" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="R18" s="3">
+      <c r="S18" s="3">
         <v>13</v>
       </c>
-      <c r="S18" s="9" t="s">
+      <c r="T18" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="T18" s="2" t="s">
+      <c r="U18" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="U18" s="2">
-        <v>1</v>
-      </c>
-      <c r="V18" s="9" t="s">
+      <c r="V18" s="2">
+        <v>1</v>
+      </c>
+      <c r="W18" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="W18" s="2">
+      <c r="X18" s="2">
         <v>0.51</v>
       </c>
-      <c r="X18" s="2">
+      <c r="Y18" s="2">
         <v>0.32</v>
       </c>
-      <c r="Y18" s="2">
+      <c r="Z18" s="2">
         <v>0.82</v>
       </c>
-      <c r="Z18" s="17">
+      <c r="AA18" s="17">
         <f>0.212487306783715*(0.88)</f>
         <v>0.1869888299696692</v>
       </c>
+      <c r="AB18" s="17"/>
     </row>
-    <row r="19" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="18">
         <v>18</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="18">
+        <v>1</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="9" t="s">
+      <c r="D19" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="F19" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="F19" s="9">
+      <c r="G19" s="9">
         <v>0.8</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="H19" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="H19" s="9">
+      <c r="I19" s="9">
         <v>0.5</v>
       </c>
-      <c r="K19" s="8">
+      <c r="K19" s="9"/>
+      <c r="L19" s="8">
         <v>285</v>
       </c>
-      <c r="L19" s="11">
+      <c r="M19" s="11">
         <v>3.5904528499278272</v>
       </c>
-      <c r="M19" s="7">
+      <c r="N19" s="7">
         <v>12089034.749908645</v>
       </c>
-      <c r="N19" s="2">
+      <c r="O19" s="2">
         <v>2</v>
       </c>
-      <c r="O19" s="2">
-        <v>1</v>
-      </c>
       <c r="P19" s="2">
         <v>1</v>
       </c>
-      <c r="Q19" s="4" t="s">
+      <c r="Q19" s="2">
+        <v>1</v>
+      </c>
+      <c r="R19" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="R19" s="5" t="s">
+      <c r="S19" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="S19" s="9" t="s">
+      <c r="T19" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="T19" s="4" t="s">
+      <c r="U19" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="U19" s="2">
-        <v>1</v>
-      </c>
-      <c r="V19" s="2" t="s">
+      <c r="V19" s="2">
+        <v>1</v>
+      </c>
+      <c r="W19" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="W19" s="2">
+      <c r="X19" s="2">
         <v>0.81</v>
       </c>
-      <c r="X19" s="2">
+      <c r="Y19" s="2">
         <v>0.51</v>
       </c>
-      <c r="Y19" s="2">
+      <c r="Z19" s="2">
         <v>1.3</v>
       </c>
-      <c r="Z19" s="17">
+      <c r="AA19" s="17">
         <f>0.8*(0.88)</f>
         <v>0.70400000000000007</v>
       </c>
+      <c r="AB19" s="17"/>
     </row>
-    <row r="20" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="F20" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="F20" s="2">
+      <c r="G20" s="2">
         <v>0.05</v>
       </c>
-      <c r="G20" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="H20" s="2">
+      <c r="I20" s="2">
         <v>0.05</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="J20" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="J20" s="2">
+      <c r="K20" s="2">
         <v>0.05</v>
       </c>
-      <c r="K20" s="8">
+      <c r="L20" s="8">
         <v>380</v>
       </c>
-      <c r="L20" s="11">
+      <c r="M20" s="11">
         <v>1.2581054540850005</v>
       </c>
-      <c r="M20" s="7">
+      <c r="N20" s="7">
         <v>87661.259262234264</v>
       </c>
-      <c r="N20" s="2">
+      <c r="O20" s="2">
         <v>2</v>
       </c>
-      <c r="O20" s="2">
-        <v>1</v>
-      </c>
       <c r="P20" s="2">
         <v>1</v>
       </c>
-      <c r="Q20" s="2" t="s">
+      <c r="Q20" s="2">
+        <v>1</v>
+      </c>
+      <c r="R20" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="R20" s="3">
+      <c r="S20" s="3">
         <v>11</v>
       </c>
-      <c r="S20" s="2" t="s">
+      <c r="T20" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="T20" s="2" t="s">
+      <c r="U20" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="U20" s="2">
-        <v>1</v>
-      </c>
-      <c r="V20" s="2" t="s">
+      <c r="V20" s="2">
+        <v>1</v>
+      </c>
+      <c r="W20" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="W20" s="2">
+      <c r="X20" s="2">
         <v>0.6</v>
       </c>
-      <c r="X20" s="2">
+      <c r="Y20" s="2">
         <v>0.44</v>
       </c>
-      <c r="Y20" s="2">
+      <c r="Z20" s="2">
         <v>0.81</v>
       </c>
-      <c r="Z20" s="17">
+      <c r="AA20" s="17">
         <f>0.1*(0.88)</f>
         <v>8.8000000000000009E-2</v>
       </c>
+      <c r="AB20" s="17"/>
     </row>
-    <row r="21" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="18">
         <v>20</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="18">
+        <v>1</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="F21" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="F21" s="2">
+      <c r="G21" s="2">
         <v>0.2</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="H21" s="2">
+      <c r="I21" s="2">
         <v>0.2</v>
       </c>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2">
+      <c r="K21" s="2"/>
+      <c r="L21" s="2">
         <v>437</v>
       </c>
-      <c r="L21" s="11">
+      <c r="M21" s="11">
         <v>21.299447386134773</v>
       </c>
-      <c r="M21" s="7">
+      <c r="N21" s="7">
         <v>10246902.750900846</v>
       </c>
-      <c r="N21" s="2">
+      <c r="O21" s="2">
         <v>3</v>
       </c>
-      <c r="O21" s="2">
-        <v>1</v>
-      </c>
       <c r="P21" s="2">
         <v>1</v>
       </c>
-      <c r="Q21" s="2" t="s">
+      <c r="Q21" s="2">
+        <v>1</v>
+      </c>
+      <c r="R21" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="R21" s="3">
+      <c r="S21" s="3">
         <v>13</v>
       </c>
-      <c r="S21" s="2" t="s">
+      <c r="T21" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="T21" s="2" t="s">
+      <c r="U21" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="U21" s="2">
-        <v>1</v>
-      </c>
-      <c r="V21" s="2" t="s">
+      <c r="V21" s="2">
+        <v>1</v>
+      </c>
+      <c r="W21" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="W21" s="2">
+      <c r="X21" s="2">
         <v>1.49</v>
       </c>
-      <c r="X21" s="2">
+      <c r="Y21" s="2">
         <v>1.29</v>
       </c>
-      <c r="Y21" s="2">
+      <c r="Z21" s="2">
         <v>1.72</v>
       </c>
-      <c r="Z21" s="17">
+      <c r="AA21" s="17">
         <f>0.212487306783715*(0.88)</f>
         <v>0.1869888299696692</v>
       </c>
+      <c r="AB21" s="17"/>
     </row>
-    <row r="22" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="F22" s="2">
+      <c r="G22" s="2">
         <v>0.85</v>
       </c>
-      <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
-      <c r="K22" s="2">
+      <c r="K22" s="2"/>
+      <c r="L22" s="2">
         <v>440.3</v>
       </c>
-      <c r="L22" s="11">
+      <c r="M22" s="11">
         <v>1.1496900605005875</v>
       </c>
-      <c r="M22" s="7">
+      <c r="N22" s="7">
         <v>864625.4042493247</v>
       </c>
-      <c r="N22" s="2">
+      <c r="O22" s="2">
         <v>5</v>
       </c>
-      <c r="O22" s="2">
+      <c r="P22" s="2">
         <v>2</v>
       </c>
-      <c r="P22" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="2" t="s">
+      <c r="Q22" s="2">
+        <v>1</v>
+      </c>
+      <c r="R22" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="R22" s="3">
+      <c r="S22" s="3">
         <v>18</v>
       </c>
-      <c r="S22" s="2" t="s">
+      <c r="T22" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="T22" s="2" t="s">
+      <c r="U22" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="U22" s="7">
-        <v>1</v>
-      </c>
-      <c r="V22" s="2" t="s">
+      <c r="V22" s="7">
+        <v>1</v>
+      </c>
+      <c r="W22" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="W22" s="2">
+      <c r="X22" s="2">
         <v>0.96199999999999997</v>
       </c>
-      <c r="X22" s="2">
+      <c r="Y22" s="2">
         <v>0.80400000000000005</v>
       </c>
-      <c r="Y22" s="2">
+      <c r="Z22" s="2">
         <v>0.999</v>
       </c>
-      <c r="Z22" s="17">
+      <c r="AA22" s="17">
         <f>0.924908816360775*(0.88)</f>
         <v>0.8139197583974821</v>
       </c>
+      <c r="AB22" s="17"/>
     </row>
-    <row r="23" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="18">
         <v>22</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="18">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="9" t="s">
+      <c r="F23" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="F23" s="2">
+      <c r="G23" s="2">
         <v>0.05</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="H23" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="H23" s="2">
+      <c r="I23" s="2">
         <v>0.2</v>
       </c>
-      <c r="J23" s="2"/>
-      <c r="K23" s="8">
+      <c r="K23" s="2"/>
+      <c r="L23" s="8">
         <v>566</v>
       </c>
-      <c r="L23" s="11">
+      <c r="M23" s="11">
         <v>1.2581054540850005</v>
       </c>
-      <c r="M23" s="7">
+      <c r="N23" s="7">
         <v>284844.82375269063</v>
       </c>
-      <c r="Q23" s="2" t="s">
+      <c r="R23" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="R23" s="3">
+      <c r="S23" s="3">
         <v>20</v>
       </c>
-      <c r="S23" s="2" t="s">
+      <c r="T23" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="T23" s="2" t="s">
+      <c r="U23" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="U23" s="2">
-        <v>1</v>
-      </c>
-      <c r="V23" s="2" t="s">
+      <c r="V23" s="2">
+        <v>1</v>
+      </c>
+      <c r="W23" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="W23" s="2">
+      <c r="X23" s="2">
         <v>-0.25</v>
       </c>
-      <c r="X23" s="2">
+      <c r="Y23" s="2">
         <v>-0.5</v>
       </c>
-      <c r="Y23" s="2">
+      <c r="Z23" s="2">
         <v>0</v>
       </c>
-      <c r="Z23" s="17">
+      <c r="AA23" s="17">
         <f>0.1*(0.88)</f>
         <v>8.8000000000000009E-2</v>
       </c>
+      <c r="AB23" s="17"/>
     </row>
-    <row r="24" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="F24" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="F24" s="2">
+      <c r="G24" s="2">
         <v>0.3</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="H24" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="H24" s="2">
+      <c r="I24" s="2">
         <v>0.05</v>
       </c>
-      <c r="J24" s="2"/>
-      <c r="K24" s="8">
+      <c r="K24" s="2"/>
+      <c r="L24" s="8">
         <v>576</v>
       </c>
-      <c r="L24" s="11">
+      <c r="M24" s="11">
         <v>1.6278196387318138</v>
       </c>
-      <c r="M24" s="7">
+      <c r="N24" s="7">
         <v>2087282.1552937152</v>
       </c>
-      <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
-      <c r="Q24" s="4" t="s">
+      <c r="Q24" s="1"/>
+      <c r="R24" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="R24" s="5" t="s">
+      <c r="S24" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="S24" s="2" t="s">
+      <c r="T24" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="T24" s="4" t="s">
+      <c r="U24" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="U24" s="2">
-        <v>1</v>
-      </c>
-      <c r="V24" s="2" t="s">
+      <c r="V24" s="2">
+        <v>1</v>
+      </c>
+      <c r="W24" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="W24" s="2" t="s">
+      <c r="X24" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="X24" s="2">
+      <c r="Y24" s="2">
         <v>1.18</v>
       </c>
-      <c r="Y24" s="2">
+      <c r="Z24" s="2">
         <v>2.59</v>
       </c>
-      <c r="Z24" s="17">
+      <c r="AA24" s="17">
         <f>0.322446666744185*(0.88)</f>
         <v>0.28375306673488276</v>
       </c>
+      <c r="AB24" s="17"/>
     </row>
-    <row r="25" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="18">
         <v>24</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="18">
+        <v>1</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="D25" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F25" s="2">
+      <c r="G25" s="2">
         <v>0.2</v>
       </c>
-      <c r="G25" s="2"/>
       <c r="H25" s="2"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="8">
+      <c r="I25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="8">
         <v>624</v>
       </c>
-      <c r="L25" s="11">
+      <c r="M25" s="11">
         <v>0.92177949382319446</v>
       </c>
-      <c r="M25" s="7">
+      <c r="N25" s="7">
         <v>168.48926117059352</v>
       </c>
-      <c r="P25" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q25" s="2" t="s">
+      <c r="Q25" s="2">
+        <v>1</v>
+      </c>
+      <c r="R25" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="R25" s="3" t="s">
+      <c r="S25" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="S25" s="9" t="s">
+      <c r="T25" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="T25" s="2" t="s">
+      <c r="U25" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="U25" s="2">
-        <v>1</v>
-      </c>
-      <c r="V25" s="10"/>
-      <c r="Z25" s="17">
+      <c r="V25" s="2">
+        <v>1</v>
+      </c>
+      <c r="W25" s="10"/>
+      <c r="Z25" s="2"/>
+      <c r="AA25" s="17">
         <f>0.1*(0.88)</f>
         <v>8.8000000000000009E-2</v>
       </c>
+      <c r="AB25" s="17"/>
     </row>
-    <row r="26" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="2">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="F26" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="2">
+      <c r="G26" s="2">
         <v>0.6</v>
       </c>
-      <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="2"/>
-      <c r="K26" s="2">
+      <c r="K26" s="2"/>
+      <c r="L26" s="2">
         <v>1186</v>
       </c>
-      <c r="L26" s="11">
+      <c r="M26" s="11">
         <v>0.248529494536535</v>
       </c>
-      <c r="M26" s="7">
+      <c r="N26" s="7">
         <v>357.06339814683844</v>
       </c>
-      <c r="N26" s="2">
+      <c r="O26" s="2">
         <v>2</v>
       </c>
-      <c r="O26" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q26" s="2" t="s">
+      <c r="P26" s="2">
+        <v>1</v>
+      </c>
+      <c r="R26" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="R26" s="3" t="s">
+      <c r="S26" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="S26" s="2" t="s">
+      <c r="T26" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="T26" s="2" t="s">
+      <c r="U26" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="U26" s="2">
-        <v>1</v>
-      </c>
-      <c r="V26" s="2"/>
-      <c r="Z26" s="17">
+      <c r="V26" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="2"/>
+      <c r="AA26" s="17">
         <v>0.4</v>
       </c>
+      <c r="AB26" s="17"/>
     </row>
-    <row r="27" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="18">
         <v>26</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="18">
+        <v>1</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="D27" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="F27" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="F27" s="2">
+      <c r="G27" s="2">
         <v>0.8</v>
       </c>
-      <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
-      <c r="K27" s="8">
+      <c r="K27" s="2"/>
+      <c r="L27" s="8">
         <v>1830</v>
       </c>
-      <c r="L27" s="11">
+      <c r="M27" s="11">
         <v>0.26010121047192036</v>
       </c>
-      <c r="M27" s="7">
+      <c r="N27" s="7">
         <v>39.434643534151753</v>
       </c>
-      <c r="N27" s="2">
-        <v>1</v>
-      </c>
       <c r="O27" s="2">
+        <v>1</v>
+      </c>
+      <c r="P27" s="2">
         <v>3</v>
       </c>
-      <c r="P27" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q27" s="2" t="s">
+      <c r="Q27" s="2">
+        <v>1</v>
+      </c>
+      <c r="R27" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="R27" s="3" t="s">
+      <c r="S27" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="S27" s="9" t="s">
+      <c r="T27" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="T27" s="2" t="s">
+      <c r="U27" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="U27" s="2">
-        <v>1</v>
-      </c>
-      <c r="V27" s="12" t="s">
+      <c r="V27" s="2">
+        <v>1</v>
+      </c>
+      <c r="W27" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="W27" s="2">
+      <c r="X27" s="2">
         <v>0.38</v>
       </c>
-      <c r="X27" s="2">
+      <c r="Y27" s="2">
         <v>0.27</v>
       </c>
-      <c r="Y27" s="2">
+      <c r="Z27" s="2">
         <v>0.55000000000000004</v>
       </c>
-      <c r="Z27" s="17">
+      <c r="AA27" s="17">
         <f>0.8*(0.88)</f>
         <v>0.70400000000000007</v>
       </c>
+      <c r="AB27" s="17"/>
     </row>
-    <row r="28" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="C28" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="D28" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="F28" s="2">
+      <c r="G28" s="2">
         <v>0.5</v>
       </c>
-      <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
-      <c r="K28" s="8">
+      <c r="K28" s="2"/>
+      <c r="L28" s="8">
         <v>2040</v>
       </c>
-      <c r="L28" s="11">
+      <c r="M28" s="11">
         <v>12.313176410983239</v>
       </c>
-      <c r="M28" s="7">
+      <c r="N28" s="7">
         <v>28689.751829313835</v>
       </c>
-      <c r="N28" s="2">
+      <c r="O28" s="2">
         <v>6</v>
       </c>
-      <c r="O28" s="2">
-        <v>1</v>
-      </c>
       <c r="P28" s="2">
         <v>1</v>
       </c>
-      <c r="Q28" s="2" t="s">
+      <c r="Q28" s="2">
+        <v>1</v>
+      </c>
+      <c r="R28" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="R28" s="3" t="s">
+      <c r="S28" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="S28" s="9" t="s">
+      <c r="T28" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="T28" s="2" t="s">
+      <c r="U28" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="U28" s="2">
-        <v>1</v>
-      </c>
-      <c r="V28" s="12" t="s">
+      <c r="V28" s="2">
+        <v>1</v>
+      </c>
+      <c r="W28" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="W28" s="2">
+      <c r="X28" s="2">
         <v>0.15</v>
       </c>
-      <c r="X28" s="2">
+      <c r="Y28" s="2">
         <v>0.12</v>
       </c>
-      <c r="Y28" s="2">
+      <c r="Z28" s="2">
         <v>0.32</v>
       </c>
-      <c r="Z28" s="17">
+      <c r="AA28" s="17">
         <f>0.391259294961732*(0.88)</f>
         <v>0.34430817956632415</v>
       </c>
+      <c r="AB28" s="17"/>
     </row>
-    <row r="29" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="18">
         <v>28</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="18">
+        <v>1</v>
+      </c>
+      <c r="C29" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="D29" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E29" s="9" t="s">
+      <c r="F29" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="F29" s="9">
+      <c r="G29" s="9">
         <v>0.2</v>
       </c>
-      <c r="G29" s="9" t="s">
+      <c r="H29" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="H29" s="9">
+      <c r="I29" s="9">
         <v>0.05</v>
       </c>
-      <c r="I29" s="9" t="s">
+      <c r="J29" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="J29" s="9">
+      <c r="K29" s="9">
         <v>0.1</v>
       </c>
-      <c r="K29" s="8">
+      <c r="L29" s="8">
         <v>4393</v>
       </c>
-      <c r="L29" s="11">
+      <c r="M29" s="11">
         <v>0.78435308805910964</v>
       </c>
-      <c r="M29" s="7">
+      <c r="N29" s="7">
         <v>31255.550710902706</v>
       </c>
-      <c r="N29" s="2">
+      <c r="O29" s="2">
         <v>0</v>
       </c>
-      <c r="O29" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q29" s="2" t="s">
+      <c r="P29" s="2">
+        <v>1</v>
+      </c>
+      <c r="R29" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="R29" s="3">
+      <c r="S29" s="3">
         <v>11</v>
       </c>
-      <c r="S29" s="9" t="s">
+      <c r="T29" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="T29" s="2" t="s">
+      <c r="U29" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="U29" s="2">
-        <v>1</v>
-      </c>
-      <c r="V29" s="9" t="s">
+      <c r="V29" s="2">
+        <v>1</v>
+      </c>
+      <c r="W29" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="W29" s="2">
+      <c r="X29" s="2">
         <v>7.2300000000000003E-2</v>
-      </c>
-      <c r="X29" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="Y29" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="Z29" s="17">
+      <c r="Z29" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA29" s="17">
         <f>0.210614324578582*(0.88)</f>
         <v>0.18534060562915217</v>
       </c>
+      <c r="AB29" s="17"/>
     </row>
-    <row r="30" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
+      <c r="C30" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="D30" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E30" s="9" t="s">
+      <c r="F30" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="F30" s="9">
+      <c r="G30" s="9">
         <v>0.4</v>
       </c>
-      <c r="K30" s="8">
+      <c r="K30" s="9"/>
+      <c r="L30" s="8">
         <v>5488</v>
       </c>
-      <c r="L30" s="11">
+      <c r="M30" s="11">
         <v>19.359239841281244</v>
       </c>
-      <c r="M30" s="16">
+      <c r="N30" s="16">
         <v>190292.44749432051</v>
-      </c>
-      <c r="N30" s="2">
-        <v>3</v>
       </c>
       <c r="O30" s="2">
         <v>3</v>
       </c>
       <c r="P30" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q30" s="2">
+        <v>1</v>
+      </c>
+      <c r="R30" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="R30" s="3">
-        <v>1</v>
-      </c>
-      <c r="S30" s="9" t="s">
+      <c r="S30" s="3">
+        <v>1</v>
+      </c>
+      <c r="T30" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="T30" s="2" t="s">
+      <c r="U30" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="U30" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z30" s="17">
+      <c r="V30" s="2">
+        <v>1</v>
+      </c>
+      <c r="W30" s="9"/>
+      <c r="Z30" s="2"/>
+      <c r="AA30" s="17">
         <f>0.253110379496502*(0.88)</f>
         <v>0.22273713395692177</v>
       </c>
+      <c r="AB30" s="17"/>
     </row>
-    <row r="31" spans="1:26" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="18">
         <v>30</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="18">
+        <v>1</v>
+      </c>
+      <c r="C31" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="D31" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="F31" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="F31" s="9">
+      <c r="G31" s="9">
         <v>0.2</v>
       </c>
-      <c r="G31" s="9" t="s">
+      <c r="H31" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="H31" s="9">
+      <c r="I31" s="9">
         <v>0.05</v>
       </c>
-      <c r="I31" s="9" t="s">
+      <c r="J31" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="J31" s="9">
+      <c r="K31" s="9">
         <v>0.05</v>
       </c>
-      <c r="K31" s="8">
+      <c r="L31" s="8">
         <v>11484</v>
       </c>
-      <c r="L31" s="11">
+      <c r="M31" s="11">
         <v>21.299447386134773</v>
       </c>
-      <c r="M31" s="7">
+      <c r="N31" s="7">
         <v>9111068.3478771001</v>
       </c>
-      <c r="N31" s="2">
+      <c r="O31" s="2">
         <v>2</v>
       </c>
-      <c r="O31" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q31" s="2" t="s">
+      <c r="P31" s="2">
+        <v>1</v>
+      </c>
+      <c r="R31" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="R31" s="3" t="s">
+      <c r="S31" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="S31" s="9" t="s">
+      <c r="T31" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="T31" s="2" t="s">
+      <c r="U31" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="U31" s="2">
-        <v>1</v>
-      </c>
-      <c r="V31" s="9" t="s">
+      <c r="V31" s="2">
+        <v>1</v>
+      </c>
+      <c r="W31" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="W31" s="2">
+      <c r="X31" s="2">
         <v>0.34</v>
-      </c>
-      <c r="X31" s="2" t="s">
-        <v>132</v>
       </c>
       <c r="Y31" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="Z31" s="17">
+      <c r="Z31" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="AA31" s="17">
         <f>0.212487306783715*(0.88)</f>
         <v>0.1869888299696692</v>
       </c>
+      <c r="AB31" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new version is working
</commit_message>
<xml_diff>
--- a/data/interventions-demo.xlsx
+++ b/data/interventions-demo.xlsx
@@ -21,6 +21,60 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>cliffk</author>
+  </authors>
+  <commentList>
+    <comment ref="G5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>cliffk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+Was 22</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>cliffk:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+Was 31</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="182">
   <si>
@@ -516,9 +570,6 @@
     <t>Pneumococcal meningitis: 0.4</t>
   </si>
   <si>
-    <t>Diarrheal diseases: 0.3</t>
-  </si>
-  <si>
     <t>Pneumococcal meningitis: 0.7</t>
   </si>
   <si>
@@ -561,13 +612,16 @@
     <t>Anxiety disorders: 0.2; Attention-deficit/hyperactivity disorder: 0.05; Conduct disorder: 0.05</t>
   </si>
   <si>
-    <t>HIV/AIDS: 0.05; Sexually transmitted diseases excluding HIV: 0.03; Acute hepatitis A: 0.02; Acute hepatitis E: 0.02</t>
-  </si>
-  <si>
-    <t>Sexually transmitted diseases excluding HIV: 0.2; Urinary diseases and male infertility: 0.6</t>
-  </si>
-  <si>
     <t>Ischemic heart disease: 0.05; Hemorrhagic stroke: 0.05; Ischemic stroke: 0.05</t>
+  </si>
+  <si>
+    <t>HIV/AIDS: 0.2; Sexually transmitted diseases excluding HIV: 0.1; Acute hepatitis A: 0.1; Acute hepatitis E: 0.1</t>
+  </si>
+  <si>
+    <t>Sexually transmitted diseases excluding HIV: 0.7; Urinary diseases and male infertility: 0.7</t>
+  </si>
+  <si>
+    <t>Diarrheal diseases: 0.5</t>
   </si>
 </sst>
 </file>
@@ -578,7 +632,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -657,6 +711,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2679,12 +2744,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2799,7 +2864,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G2" s="8">
         <v>576</v>
@@ -3010,7 +3075,7 @@
         <v>160</v>
       </c>
       <c r="G5" s="8">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="H5" s="11">
         <v>1.6708715227994324</v>
@@ -3070,8 +3135,7 @@
         <v>163</v>
       </c>
       <c r="G6" s="14">
-        <f>G9</f>
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="H6" s="11">
         <v>19.359239841281244</v>
@@ -3138,7 +3202,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>164</v>
+        <v>181</v>
       </c>
       <c r="G7" s="2">
         <v>95</v>
@@ -3208,7 +3272,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G8" s="2">
         <v>1186</v>
@@ -3455,7 +3519,7 @@
         <v>10</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G12" s="8">
         <v>380</v>
@@ -3525,7 +3589,7 @@
         <v>4</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G13" s="2">
         <v>437</v>
@@ -3665,7 +3729,7 @@
         <v>4</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G15" s="8">
         <v>115</v>
@@ -3735,7 +3799,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G16" s="8">
         <v>2040</v>
@@ -3875,7 +3939,7 @@
         <v>10</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G18" s="8">
         <v>5488</v>
@@ -3935,7 +3999,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G19" s="2">
         <v>440.3</v>
@@ -4075,7 +4139,7 @@
         <v>4</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G21" s="8">
         <v>4393</v>
@@ -4203,7 +4267,7 @@
         <v>0</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G23" s="2">
         <v>103</v>
@@ -4333,7 +4397,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G25" s="8">
         <v>285</v>
@@ -4403,7 +4467,7 @@
         <v>4</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G26" s="8">
         <v>11484</v>
@@ -4470,7 +4534,7 @@
         <v>4</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G27" s="8">
         <v>566</v>
@@ -4607,7 +4671,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G29" s="8">
         <v>624</v>
@@ -4737,7 +4801,7 @@
         <v>0</v>
       </c>
       <c r="F31" s="9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G31" s="8">
         <v>1830</v>
@@ -4793,8 +4857,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>